<commit_message>
finishing C3C2 part and update notes and code
</commit_message>
<xml_diff>
--- a/Chapter3/Code/datasetExample.xlsx
+++ b/Chapter3/Code/datasetExample.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michael/Documents/MDLforBeginners/Chapter3/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C640C5-DF81-0D43-99BB-D51D3BAB0EF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B80887-AF62-2B45-9C52-7BCD33487D04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{637A412D-03CE-0A45-BF4A-D8C57A98DDF1}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{637A412D-03CE-0A45-BF4A-D8C57A98DDF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="covmatrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>姓名</t>
   </si>
@@ -57,6 +58,33 @@
   </si>
   <si>
     <t>Lucy</t>
+  </si>
+  <si>
+    <t>Kara</t>
+  </si>
+  <si>
+    <t>语文</t>
+  </si>
+  <si>
+    <t>数学</t>
+  </si>
+  <si>
+    <t>英语</t>
+  </si>
+  <si>
+    <t>物理</t>
+  </si>
+  <si>
+    <t>历史</t>
+  </si>
+  <si>
+    <t>人工智能</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>Science</t>
   </si>
 </sst>
 </file>
@@ -94,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -182,11 +210,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -210,6 +346,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -528,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90FF809-E762-1145-A8DB-1105CE11078B}">
   <dimension ref="F4:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="C1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,4 +805,350 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9157597B-0680-2D4E-8208-7A36F05AE464}">
+  <dimension ref="E8:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="21">
+        <v>60</v>
+      </c>
+      <c r="H9" s="22">
+        <v>90</v>
+      </c>
+      <c r="I9" s="22">
+        <v>60</v>
+      </c>
+      <c r="J9" s="22">
+        <v>80</v>
+      </c>
+      <c r="K9" s="22">
+        <v>70</v>
+      </c>
+      <c r="L9" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="14">
+        <v>60</v>
+      </c>
+      <c r="H10" s="6">
+        <v>90</v>
+      </c>
+      <c r="I10" s="6">
+        <v>60</v>
+      </c>
+      <c r="J10" s="6">
+        <v>80</v>
+      </c>
+      <c r="K10" s="6">
+        <v>70</v>
+      </c>
+      <c r="L10" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="14">
+        <v>60</v>
+      </c>
+      <c r="H11" s="6">
+        <v>90</v>
+      </c>
+      <c r="I11" s="6">
+        <v>60</v>
+      </c>
+      <c r="J11" s="6">
+        <v>80</v>
+      </c>
+      <c r="K11" s="6">
+        <v>70</v>
+      </c>
+      <c r="L11" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="14">
+        <v>60</v>
+      </c>
+      <c r="H12" s="6">
+        <v>90</v>
+      </c>
+      <c r="I12" s="6">
+        <v>60</v>
+      </c>
+      <c r="J12" s="6">
+        <v>80</v>
+      </c>
+      <c r="K12" s="6">
+        <v>70</v>
+      </c>
+      <c r="L12" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="14">
+        <v>60</v>
+      </c>
+      <c r="H13" s="6">
+        <v>90</v>
+      </c>
+      <c r="I13" s="6">
+        <v>60</v>
+      </c>
+      <c r="J13" s="6">
+        <v>80</v>
+      </c>
+      <c r="K13" s="6">
+        <v>70</v>
+      </c>
+      <c r="L13" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="15">
+        <v>60</v>
+      </c>
+      <c r="H14" s="17">
+        <v>90</v>
+      </c>
+      <c r="I14" s="17">
+        <v>60</v>
+      </c>
+      <c r="J14" s="17">
+        <v>80</v>
+      </c>
+      <c r="K14" s="17">
+        <v>70</v>
+      </c>
+      <c r="L14" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F18" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="21">
+        <v>90</v>
+      </c>
+      <c r="H18" s="22">
+        <v>60</v>
+      </c>
+      <c r="I18" s="22">
+        <v>80</v>
+      </c>
+      <c r="J18" s="22">
+        <v>60</v>
+      </c>
+      <c r="K18" s="22">
+        <v>100</v>
+      </c>
+      <c r="L18" s="23">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="14">
+        <v>90</v>
+      </c>
+      <c r="H19" s="6">
+        <v>60</v>
+      </c>
+      <c r="I19" s="6">
+        <v>80</v>
+      </c>
+      <c r="J19" s="6">
+        <v>60</v>
+      </c>
+      <c r="K19" s="6">
+        <v>100</v>
+      </c>
+      <c r="L19" s="16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="14">
+        <v>90</v>
+      </c>
+      <c r="H20" s="6">
+        <v>60</v>
+      </c>
+      <c r="I20" s="6">
+        <v>80</v>
+      </c>
+      <c r="J20" s="6">
+        <v>60</v>
+      </c>
+      <c r="K20" s="6">
+        <v>100</v>
+      </c>
+      <c r="L20" s="16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="14">
+        <v>90</v>
+      </c>
+      <c r="H21" s="6">
+        <v>60</v>
+      </c>
+      <c r="I21" s="6">
+        <v>80</v>
+      </c>
+      <c r="J21" s="6">
+        <v>60</v>
+      </c>
+      <c r="K21" s="6">
+        <v>100</v>
+      </c>
+      <c r="L21" s="16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="14">
+        <v>90</v>
+      </c>
+      <c r="H22" s="6">
+        <v>60</v>
+      </c>
+      <c r="I22" s="6">
+        <v>80</v>
+      </c>
+      <c r="J22" s="6">
+        <v>60</v>
+      </c>
+      <c r="K22" s="6">
+        <v>100</v>
+      </c>
+      <c r="L22" s="16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="15">
+        <v>90</v>
+      </c>
+      <c r="H23" s="17">
+        <v>60</v>
+      </c>
+      <c r="I23" s="17">
+        <v>80</v>
+      </c>
+      <c r="J23" s="17">
+        <v>60</v>
+      </c>
+      <c r="K23" s="17">
+        <v>100</v>
+      </c>
+      <c r="L23" s="18">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finishing all notes for chapter 3
</commit_message>
<xml_diff>
--- a/Chapter3/Code/datasetExample.xlsx
+++ b/Chapter3/Code/datasetExample.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michael/Documents/MDLforBeginners/Chapter3/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B80887-AF62-2B45-9C52-7BCD33487D04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB03FFA5-9FE8-E443-9997-80E1F78D8BD2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{637A412D-03CE-0A45-BF4A-D8C57A98DDF1}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{637A412D-03CE-0A45-BF4A-D8C57A98DDF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="covmatrix" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>姓名</t>
   </si>
@@ -85,6 +86,30 @@
   </si>
   <si>
     <t>Science</t>
+  </si>
+  <si>
+    <t>体重</t>
+  </si>
+  <si>
+    <t>性别代码(0,1)</t>
+  </si>
+  <si>
+    <t>年龄</t>
+  </si>
+  <si>
+    <t>最近一次英语成绩(百分制)</t>
+  </si>
+  <si>
+    <t>最近一次数学成绩(百分制)</t>
+  </si>
+  <si>
+    <t>视力</t>
+  </si>
+  <si>
+    <t>一周上网的时间(小时制)</t>
+  </si>
+  <si>
+    <t>亲密朋友个数</t>
   </si>
 </sst>
 </file>
@@ -322,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -392,6 +417,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9157597B-0680-2D4E-8208-7A36F05AE464}">
   <dimension ref="E8:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1151,4 +1177,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F561E025-977A-784B-958F-C58E398CD38C}">
+  <dimension ref="G10:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G10" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G11" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finish chapter 3 with notes, exercises, and lecture handouts :)
</commit_message>
<xml_diff>
--- a/Chapter3/Code/datasetExample.xlsx
+++ b/Chapter3/Code/datasetExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michael/Documents/MDLforBeginners/Chapter3/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB03FFA5-9FE8-E443-9997-80E1F78D8BD2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7FA9BB-BBFF-984F-B685-2222EA1D48C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{637A412D-03CE-0A45-BF4A-D8C57A98DDF1}"/>
   </bookViews>
@@ -1184,7 +1184,7 @@
   <dimension ref="G10:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>